<commit_message>
#875 #857 #858 Added ability to insert nsmi codes to topics, resources. Filled the codes in existing entities
</commit_message>
<xml_diff>
--- a/Tools/Access2JusticeCode.DataImportTool/SampleFiles/Resources Importer test file.xlsx
+++ b/Tools/Access2JusticeCode.DataImportTool/SampleFiles/Resources Importer test file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-sobhad\Desktop\Clone-A2J\Access2Justice\Tools\Access2Justice.Tools.CsvImporter\SampleFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Source\Repos\LegalNavigator\Tools\Access2JusticeCode.DataImportTool\SampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E29EC5-5C34-496A-8CA0-1B52797F63ED}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7176AA53-0763-4DEB-ADC2-550C506DBFBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="6920" tabRatio="722" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description of Template" sheetId="9" r:id="rId1"/>
@@ -62,70 +62,142 @@
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Name/Title of the resources (e.g. Organization, article, video, etc.)</t>
+        </r>
       </text>
     </comment>
     <comment ref="C1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Description/overview of the resource which will display beneath the name (title) on the resource summary page and detailed page</t>
+        </r>
       </text>
     </comment>
     <comment ref="E1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     URL for the resource.  Will be the hyperlink associated with the name defined in column B (for display in the UI)</t>
+        </r>
       </text>
     </comment>
     <comment ref="F1" authorId="3" shapeId="0" xr:uid="{13A33FB7-8CC5-48FD-BB10-CC53F3EEFC5B}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Reference Topic(s) that are linked to the resource. ID will be known after initial topic import has been performed.</t>
+        </r>
       </text>
     </comment>
     <comment ref="H1" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to county of Honolulu, enter Honolulu in Location_County and HI in Location_State</t>
+        </r>
       </text>
     </comment>
     <comment ref="I1" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, if a topic applies only to a county of Honolulu, enter Honolulu in Location_County
  and HI in Location_State.  
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="J1" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to city of Aiea, enter Aiea in Location_City and HI in Location_State
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="K1" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to zip code 96701, enter 96701 in Location_Zip and HI in Location_State
  If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="L1" authorId="8" shapeId="0" xr:uid="{D4C5532F-5E1B-48CB-9998-EBE9E22422D4}">
@@ -154,53 +226,107 @@
     </comment>
     <comment ref="M1" authorId="9" shapeId="0" xr:uid="{E443C1D1-531A-46F0-A2DE-4184C19110E8}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Optional field. Provides the content curator the ability to break sections of the detailed article page into further subsections using headlines.  
 Additional headlines and related content can be added (e.g. headline 2, Content 2, etc.) by inserting additional columns to articles tab.</t>
+        </r>
       </text>
     </comment>
     <comment ref="N1" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Type of resource</t>
+        </r>
       </text>
     </comment>
     <comment ref="O1" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Optional field. Provides the content curator the ability to break sections of the detailed article page into further subsections using headlines.  
 Additional headlines and related content can be added (e.g. headline 2, Content 2, etc.) by inserting additional columns to articles tab.</t>
+        </r>
       </text>
     </comment>
     <comment ref="P1" authorId="12" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Optional field. Provides the content curator the ability to add content below each headlined section.</t>
+        </r>
       </text>
     </comment>
     <comment ref="Q1" authorId="13" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Optional field. Provides the content curator the ability to break sections of the detailed article page into further subsections using headlines.  
 Additional headlines and related content can be added (e.g. headline 2, Content 2, etc.) by inserting additional columns to articles tab.</t>
+        </r>
       </text>
     </comment>
     <comment ref="R1" authorId="14" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Optional field. Provides the content curator the ability to add content below each headlined section.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -224,78 +350,159 @@
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Name/Title of the resources (e.g. Organization, article, video, etc.)</t>
+        </r>
       </text>
     </comment>
     <comment ref="C1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Description/overview of the resource which will display beneath the name (title) on the resource summary page and detailed page</t>
+        </r>
       </text>
     </comment>
     <comment ref="E1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     URL for the resource.  Will be the hyperlink associated with the name defined in column B (for display in the UI)</t>
+        </r>
       </text>
     </comment>
     <comment ref="F1" authorId="3" shapeId="0" xr:uid="{65F6564B-3B52-46B7-BAED-1B080FA41F97}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Reference Topic(s) that are linked to the resource. ID will be known after initial topic import has been performed.</t>
+        </r>
       </text>
     </comment>
     <comment ref="H1" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to county of Honolulu, enter Honolulu in Location_County and HI in Location_State</t>
+        </r>
       </text>
     </comment>
     <comment ref="I1" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, if a topic applies only to a county of Honolulu, enter Honolulu in Location_County
  and HI in Location_State.  
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="J1" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to city of Aiea, enter Aiea in Location_City and HI in Location_State
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="K1" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to zip code 96701, enter 96701 in Location_Zip and HI in Location_State
  If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="L1" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Type of resource</t>
+        </r>
       </text>
     </comment>
     <comment ref="M1" authorId="9" shapeId="0" xr:uid="{E72A0C97-4911-41EC-8D8A-9E18A8A35911}">
@@ -342,78 +549,159 @@
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Name/Title of the resources (e.g. Organization, article, video, etc.)</t>
+        </r>
       </text>
     </comment>
     <comment ref="C1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Description/overview of the resource which will display beneath the name (title) on the resource summary page and detailed page</t>
+        </r>
       </text>
     </comment>
     <comment ref="E1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     URL for the resource.  Will be the hyperlink associated with the name defined in column B (for display in the UI)</t>
+        </r>
       </text>
     </comment>
     <comment ref="F1" authorId="3" shapeId="0" xr:uid="{ABA4504B-5E34-4847-9C1F-39D516FDF689}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Reference Topic(s) that are linked to the resource. ID will be known after initial topic import has been performed.</t>
+        </r>
       </text>
     </comment>
     <comment ref="H1" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to county of Honolulu, enter Honolulu in Location_County and HI in Location_State</t>
+        </r>
       </text>
     </comment>
     <comment ref="I1" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, if a topic applies only to a county of Honolulu, enter Honolulu in Location_County
  and HI in Location_State.  
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="J1" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0400-000008000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to city of Aiea, enter Aiea in Location_City and HI in Location_State
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="K1" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0400-000009000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to zip code 96701, enter 96701 in Location_Zip and HI in Location_State
  If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="M1" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Type of resource</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -434,62 +722,125 @@
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Name/Title of the resources (e.g. Organization, article, video, etc.)</t>
+        </r>
       </text>
     </comment>
     <comment ref="C1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Description/overview of the resource which will display beneath the name (title) on the resource summary page and detailed page</t>
+        </r>
       </text>
     </comment>
     <comment ref="H1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to county of Honolulu, enter Honolulu in Location_County and HI in Location_State</t>
+        </r>
       </text>
     </comment>
     <comment ref="I1" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, if a topic applies only to a county of Honolulu, enter Honolulu in Location_County
  and HI in Location_State.  
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="J1" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to city of Aiea, enter Aiea in Location_City and HI in Location_State
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="K1" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to zip code 96701, enter 96701 in Location_Zip and HI in Location_State
  If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="N1" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Type of resource</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -515,34 +866,70 @@
   <commentList>
     <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Name/Title of the resources (e.g. Organization, article, video, etc.)</t>
+        </r>
       </text>
     </comment>
     <comment ref="C1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Description/overview of the resource which will display beneath the name (title) on the resource summary page and detailed page</t>
+        </r>
       </text>
     </comment>
     <comment ref="E1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     URL for the resource.  Will be the hyperlink associated with the name defined in column B (for display in the UI)</t>
+        </r>
       </text>
     </comment>
     <comment ref="F1" authorId="3" shapeId="0" xr:uid="{592EDAFA-D5AF-4C1A-AB66-948C7CF678D1}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Reference Topic(s) that are linked to the resource. ID will be known after initial topic import has been performed.</t>
+        </r>
       </text>
     </comment>
     <comment ref="G1" authorId="4" shapeId="0" xr:uid="{01E37D4F-FCE9-4019-B950-CBD349FB54EC}">
@@ -571,62 +958,125 @@
     </comment>
     <comment ref="H1" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to county of Honolulu, enter Honolulu in Location_County and HI in Location_State</t>
+        </r>
       </text>
     </comment>
     <comment ref="I1" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, if a topic applies only to a county of Honolulu, enter Honolulu in Location_County
  and HI in Location_State.  
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="J1" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to city of Aiea, enter Aiea in Location_City and HI in Location_State
 If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="K1" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Indicate location(s) hierarchy. Most resources will be state-wide, but some may apply to specific county / city or zip codes. For example, it a topic applies only to zip code 96701, enter 96701 in Location_Zip and HI in Location_State
  If multiple locations apply, use a pipe delimiter to delineate between locations (" | ")</t>
+        </r>
       </text>
     </comment>
     <comment ref="N1" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Phone number associated with the organization</t>
+        </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="Q1" authorId="10" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Description of who can qualify for services offered.</t>
+        </r>
       </text>
     </comment>
     <comment ref="M2" authorId="11" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Address associated with the organization</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -644,34 +1094,70 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{ECC2036D-997C-4DAE-878E-0E712CEF0307}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     This Org name should correspond to the Name cell in the Organizations tab, column B, to ensure the right review displays on the organizations page on the site.</t>
+        </r>
       </text>
     </comment>
     <comment ref="B1" authorId="1" shapeId="0" xr:uid="{252B36AE-C231-49CA-851C-B5B38AB2AB36}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Reviewers name for the said organization.</t>
+        </r>
       </text>
     </comment>
     <comment ref="C1" authorId="2" shapeId="0" xr:uid="{798560FD-4347-4F1A-8502-BE591714AEB4}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Optional field: title of the reviewer to display with the review.  Title would provide credibility for the review provided.</t>
+        </r>
       </text>
     </comment>
     <comment ref="E1" authorId="3" shapeId="0" xr:uid="{518C69C7-0CFF-43E0-A85A-C00751DFA98E}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Image of reviewer if they would like to share a photo.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -687,18 +1173,36 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     Name of the topic that will show up in the topic list</t>
+        </r>
       </text>
     </comment>
     <comment ref="B1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 This threaded comment can be viewed, but not edited in your version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924.
 Comment:
     GUID will be assigned by the development team after import, no need to enter it manually. GUIDs will be used to relate resources to topics.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -706,7 +1210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="381">
   <si>
     <t>File will be exported and cannot accommodate anything other than text (e.g. comments, pictures, etc).</t>
   </si>
@@ -1435,16 +1939,7 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Resource Type*</t>
-  </si>
-  <si>
     <t>Icon</t>
-  </si>
-  <si>
-    <t>Reviewer Title</t>
-  </si>
-  <si>
-    <t>Reviewer Image</t>
   </si>
   <si>
     <t>Overview</t>
@@ -1797,12 +2292,6 @@
     <t>Organization*</t>
   </si>
   <si>
-    <t>Reviewer Full Name*</t>
-  </si>
-  <si>
-    <t>Review Text*</t>
-  </si>
-  <si>
     <t>Comedy</t>
   </si>
   <si>
@@ -1810,13 +2299,91 @@
   </si>
   <si>
     <t>Rock</t>
+  </si>
+  <si>
+    <t>NsmiV2Code</t>
+  </si>
+  <si>
+    <t>Resource_Type*</t>
+  </si>
+  <si>
+    <t>oo-01-00-00-00</t>
+  </si>
+  <si>
+    <t>oo-02-00-00-00</t>
+  </si>
+  <si>
+    <t>oo-03-00-00-00</t>
+  </si>
+  <si>
+    <t>ff-01-00-00-00</t>
+  </si>
+  <si>
+    <t>ff-02-00-00-00</t>
+  </si>
+  <si>
+    <t>ff-03-00-00-00</t>
+  </si>
+  <si>
+    <t>rr-02-00-00-00</t>
+  </si>
+  <si>
+    <t>rr-01-00-00-00</t>
+  </si>
+  <si>
+    <t>vv-01-00-00-00</t>
+  </si>
+  <si>
+    <t>vv-02-00-00-00</t>
+  </si>
+  <si>
+    <t>aa-01-00-00-00</t>
+  </si>
+  <si>
+    <t>aa-02-00-00-00</t>
+  </si>
+  <si>
+    <t>aa-03-00-00-00</t>
+  </si>
+  <si>
+    <t>aa-04-00-00-00</t>
+  </si>
+  <si>
+    <t>or-01-00-00-00</t>
+  </si>
+  <si>
+    <t>or-02-00-00-00</t>
+  </si>
+  <si>
+    <t>or-03-00-00-00</t>
+  </si>
+  <si>
+    <t>Specialties</t>
+  </si>
+  <si>
+    <t>Qualifications</t>
+  </si>
+  <si>
+    <t>Business_Hours</t>
+  </si>
+  <si>
+    <t>Reviewer_Full_Name*</t>
+  </si>
+  <si>
+    <t>Reviewer_Title</t>
+  </si>
+  <si>
+    <t>Review_Text*</t>
+  </si>
+  <si>
+    <t>Reviewer_Image_URL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1890,6 +2457,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1993,7 +2566,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2122,6 +2695,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2657,17 +3233,17 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="131.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="131.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" ht="105" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2680,39 +3256,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="S2" sqref="S2:S5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="39" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1796875" customWidth="1"/>
-    <col min="13" max="13" width="20.26953125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" style="4" customWidth="1"/>
     <col min="14" max="14" width="26" style="1" customWidth="1"/>
-    <col min="15" max="15" width="20.26953125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" style="4" customWidth="1"/>
     <col min="16" max="16" width="34" style="4" customWidth="1"/>
-    <col min="17" max="17" width="23.54296875" style="4" customWidth="1"/>
-    <col min="18" max="18" width="37.7265625" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="9.1796875" style="3"/>
+    <col min="17" max="17" width="23.5703125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="37.7109375" style="4" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>240</v>
       </c>
@@ -2723,7 +3299,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>241</v>
+        <v>356</v>
       </c>
       <c r="E1" s="35" t="s">
         <v>3</v>
@@ -2732,7 +3308,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H1" s="35" t="s">
         <v>5</v>
@@ -2747,201 +3323,216 @@
         <v>8</v>
       </c>
       <c r="L1" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="M1" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="M1" s="37" t="s">
-        <v>245</v>
-      </c>
       <c r="N1" s="35" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="O1" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="P1" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q1" s="37" t="s">
+        <v>334</v>
+      </c>
+      <c r="R1" s="37" t="s">
         <v>335</v>
       </c>
-      <c r="P1" s="37" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>337</v>
-      </c>
-      <c r="R1" s="37" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="42" customFormat="1" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="S1" s="46" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="42" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
       <c r="B2" s="43" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I2" s="39"/>
       <c r="J2" s="39"/>
       <c r="K2" s="39"/>
       <c r="L2" s="39"/>
       <c r="M2" s="41" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="N2" s="39" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="O2" s="41" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="P2" s="41" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="Q2" s="41"/>
       <c r="R2" s="41"/>
-    </row>
-    <row r="3" spans="1:18" s="42" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+      <c r="S2" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="42" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="38"/>
       <c r="B3" s="43" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I3" s="39"/>
       <c r="J3" s="39"/>
       <c r="K3" s="39"/>
       <c r="L3" s="39"/>
       <c r="M3" s="41" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="N3" s="39" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="O3" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="P3" s="41" t="s">
         <v>265</v>
       </c>
-      <c r="P3" s="41" t="s">
-        <v>268</v>
-      </c>
       <c r="Q3" s="41" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="R3" s="41" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" s="42" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="38"/>
       <c r="B4" s="43" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H4" s="39" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I4" s="39"/>
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
       <c r="L4" s="39"/>
       <c r="M4" s="41" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="N4" s="39" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="O4" s="41" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="P4" s="41" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="Q4" s="41"/>
       <c r="R4" s="41"/>
-    </row>
-    <row r="5" spans="1:18" s="42" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="S4" s="4" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="42" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="38"/>
       <c r="B5" s="43" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G5" s="39" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I5" s="39"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
       <c r="M5" s="41" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="N5" s="39" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="O5" s="41" t="s">
+        <v>291</v>
+      </c>
+      <c r="P5" s="41" t="s">
         <v>294</v>
       </c>
-      <c r="P5" s="41" t="s">
-        <v>297</v>
-      </c>
       <c r="Q5" s="41" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="R5" s="41" t="s">
-        <v>299</v>
+        <v>296</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -2958,32 +3549,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="39" style="16" customWidth="1"/>
-    <col min="3" max="3" width="36.54296875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" style="16" customWidth="1"/>
     <col min="4" max="4" width="19" style="16" customWidth="1"/>
-    <col min="5" max="5" width="40.7265625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.54296875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="17" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.26953125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="12.1796875" customWidth="1"/>
-    <col min="14" max="14" width="24.453125" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="3"/>
+    <col min="5" max="5" width="40.7109375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.5703125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="17" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>240</v>
       </c>
@@ -2994,7 +3585,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>241</v>
+        <v>356</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>3</v>
@@ -3003,7 +3594,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>5</v>
@@ -3018,84 +3609,94 @@
         <v>8</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="M1" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="N1" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="N1" s="45" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="O1" s="46" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="25" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>339</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>320</v>
-      </c>
       <c r="G2" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
       <c r="L2" s="25" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="M2" s="39"/>
       <c r="N2" s="27" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="25" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
       <c r="L3" s="25" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="M3" s="39"/>
       <c r="N3" s="27" t="s">
-        <v>345</v>
+        <v>342</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E49" r:id="rId1" display="http://youtu.be/xJVEoCjX53M" xr:uid="{00000000-0004-0000-0300-000021000000}"/>
     <hyperlink ref="E48" r:id="rId2" display="http://youtu.be/MOcXX3csYtM" xr:uid="{00000000-0004-0000-0300-000020000000}"/>
@@ -3153,31 +3754,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="3"/>
-    <col min="2" max="2" width="27.54296875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="27.5703125" style="13" customWidth="1"/>
     <col min="3" max="3" width="48" style="13" customWidth="1"/>
-    <col min="4" max="4" width="16.90625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="40.7265625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.81640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.7265625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="3"/>
-    <col min="13" max="13" width="20.453125" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="3"/>
+    <col min="4" max="4" width="16.85546875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" style="16" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="3"/>
+    <col min="13" max="13" width="20.42578125" style="13" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>240</v>
       </c>
@@ -3188,7 +3789,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>241</v>
+        <v>356</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>3</v>
@@ -3197,7 +3798,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>5</v>
@@ -3212,72 +3813,81 @@
         <v>8</v>
       </c>
       <c r="L1" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+        <v>315</v>
+      </c>
+      <c r="N1" s="46" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="25" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
       <c r="L2" s="24"/>
       <c r="M2" s="25" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="25" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="25" t="s">
-        <v>324</v>
+        <v>321</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3305,31 +3915,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="14"/>
+    <col min="1" max="1" width="9.140625" style="14"/>
     <col min="2" max="2" width="39" style="13" customWidth="1"/>
-    <col min="3" max="3" width="36.54296875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.26953125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.26953125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="16" customWidth="1"/>
     <col min="8" max="8" width="15" style="14" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.1796875" style="3"/>
-    <col min="14" max="14" width="19.26953125" style="13" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="3"/>
+    <col min="9" max="9" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="19.28515625" style="13" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>240</v>
       </c>
@@ -3340,7 +3950,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>241</v>
+        <v>356</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>3</v>
@@ -3349,7 +3959,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>5</v>
@@ -3364,116 +3974,142 @@
         <v>8</v>
       </c>
       <c r="L1" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="M1" s="32" t="s">
         <v>242</v>
       </c>
-      <c r="M1" s="32" t="s">
-        <v>245</v>
-      </c>
       <c r="N1" s="19" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+        <v>315</v>
+      </c>
+      <c r="O1" s="46" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="22" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
       <c r="L2" s="24"/>
       <c r="M2" s="24" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
       <c r="B3" s="22" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
       <c r="L3" s="24"/>
       <c r="M3" s="24" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="N3" s="22" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>344</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
       <c r="B4" s="22" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="24"/>
       <c r="M4" s="24" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>348</v>
-      </c>
+        <v>345</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M4" xr:uid="{7C483CA7-F3FA-4825-B37A-4068E72C8EE8}"/>
@@ -3492,7 +4128,7 @@
           <x14:formula1>
             <xm:f>'Topics &amp; GUIDs reference sheet'!$D$2:$D$84</xm:f>
           </x14:formula1>
-          <xm:sqref>G13:G74</xm:sqref>
+          <xm:sqref>G12:G73</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3502,33 +4138,37 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="16"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
     <col min="2" max="2" width="25" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.54296875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="17.6328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.81640625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="15.26953125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.26953125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.26953125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="30.54296875" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.26953125" style="13" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" style="16" customWidth="1"/>
-    <col min="16" max="16" width="20.54296875" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25" style="16" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="13"/>
+    <col min="3" max="3" width="36.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="30.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="16" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="3"/>
+    <col min="17" max="17" width="20.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.140625" style="3"/>
+    <col min="20" max="20" width="25" style="16" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="15" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" s="15" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>240</v>
       </c>
@@ -3539,7 +4179,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>241</v>
+        <v>356</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>3</v>
@@ -3548,7 +4188,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>5</v>
@@ -3563,7 +4203,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M1" s="20" t="s">
         <v>9</v>
@@ -3572,138 +4212,173 @@
         <v>10</v>
       </c>
       <c r="O1" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="P1" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="P1" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="U1" s="18"/>
-    </row>
-    <row r="2" spans="1:21" ht="125.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="R1" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="S1" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="U1" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="X1" s="18"/>
+    </row>
+    <row r="2" spans="1:24" ht="125.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="22" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="21"/>
       <c r="K2" s="22"/>
       <c r="L2" s="22"/>
       <c r="M2" s="22" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O2" s="22"/>
-      <c r="P2" s="22" t="s">
-        <v>253</v>
-      </c>
+      <c r="P2" s="24"/>
       <c r="Q2" s="22" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" s="25" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
       <c r="L3" s="22"/>
       <c r="M3" s="25" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="N3" s="25" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="O3" s="25"/>
-      <c r="P3" s="25" t="s">
-        <v>259</v>
-      </c>
+      <c r="P3" s="24"/>
       <c r="Q3" s="25" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>256</v>
+      </c>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
       <c r="B4" s="25" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="22"/>
       <c r="M4" s="25" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="N4" s="25" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="O4" s="25"/>
-      <c r="P4" s="25" t="s">
-        <v>287</v>
-      </c>
+      <c r="P4" s="24"/>
       <c r="Q4" s="25" t="s">
-        <v>327</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="P5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3719,85 +4394,99 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73AA206A-4BD2-4DC7-BE0A-983E015F8CAF}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.36328125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="39.6328125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="79.453125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="79.42578125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B1" s="30" t="s">
+        <v>377</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="F1" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>243</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>356</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>334</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>328</v>
-      </c>
-      <c r="E2" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="44" t="s">
-        <v>249</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>331</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>333</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>332</v>
-      </c>
       <c r="E3" s="23" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B4" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>341</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>343</v>
+      <c r="F4" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -3832,16 +4521,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="72.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.1796875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="45.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -3855,7 +4544,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>219</v>
       </c>
@@ -3869,7 +4558,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
@@ -3883,7 +4572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -3897,7 +4586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -3911,7 +4600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -3925,7 +4614,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
@@ -3939,7 +4628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -3953,13 +4642,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>52</v>
       </c>
@@ -3973,7 +4662,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -3987,7 +4676,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -4001,7 +4690,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -4015,7 +4704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -4029,7 +4718,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>64</v>
       </c>
@@ -4044,7 +4733,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>67</v>
       </c>
@@ -4052,7 +4741,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>220</v>
       </c>
@@ -4066,7 +4755,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>70</v>
       </c>
@@ -4080,7 +4769,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>73</v>
       </c>
@@ -4094,7 +4783,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -4108,7 +4797,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
@@ -4122,7 +4811,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>67</v>
       </c>
@@ -4130,7 +4819,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>82</v>
       </c>
@@ -4144,7 +4833,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>85</v>
       </c>
@@ -4158,7 +4847,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -4172,7 +4861,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>89</v>
       </c>
@@ -4186,7 +4875,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>92</v>
       </c>
@@ -4200,7 +4889,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>95</v>
       </c>
@@ -4214,7 +4903,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>67</v>
       </c>
@@ -4222,7 +4911,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>221</v>
       </c>
@@ -4236,7 +4925,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>100</v>
       </c>
@@ -4250,7 +4939,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>102</v>
       </c>
@@ -4264,7 +4953,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>105</v>
       </c>
@@ -4278,7 +4967,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>107</v>
       </c>
@@ -4292,7 +4981,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>110</v>
       </c>
@@ -4306,7 +4995,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
       <c r="C36" t="s">
         <v>67</v>
@@ -4315,7 +5004,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>222</v>
       </c>
@@ -4329,7 +5018,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>115</v>
       </c>
@@ -4343,7 +5032,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>117</v>
       </c>
@@ -4357,7 +5046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>119</v>
       </c>
@@ -4371,7 +5060,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>122</v>
       </c>
@@ -4385,7 +5074,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>125</v>
       </c>
@@ -4399,7 +5088,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>127</v>
       </c>
@@ -4413,7 +5102,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
@@ -4427,7 +5116,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>133</v>
       </c>
@@ -4441,7 +5130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>67</v>
       </c>
@@ -4449,7 +5138,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>223</v>
       </c>
@@ -4463,7 +5152,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>137</v>
       </c>
@@ -4477,7 +5166,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>140</v>
       </c>
@@ -4491,7 +5180,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>142</v>
       </c>
@@ -4505,7 +5194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>82</v>
       </c>
@@ -4519,7 +5208,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>146</v>
       </c>
@@ -4533,7 +5222,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>64</v>
       </c>
@@ -4547,7 +5236,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>151</v>
       </c>
@@ -4561,7 +5250,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>67</v>
       </c>
@@ -4569,7 +5258,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>154</v>
       </c>
@@ -4583,7 +5272,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>157</v>
       </c>
@@ -4597,7 +5286,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>160</v>
       </c>
@@ -4611,7 +5300,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>163</v>
       </c>
@@ -4625,7 +5314,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>67</v>
       </c>
@@ -4633,7 +5322,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>225</v>
       </c>
@@ -4647,7 +5336,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>73</v>
       </c>
@@ -4661,7 +5350,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>170</v>
       </c>
@@ -4675,7 +5364,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>173</v>
       </c>
@@ -4689,7 +5378,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>175</v>
       </c>
@@ -4703,7 +5392,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>178</v>
       </c>
@@ -4717,7 +5406,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>67</v>
       </c>
@@ -4725,7 +5414,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>224</v>
       </c>
@@ -4739,7 +5428,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>183</v>
       </c>
@@ -4753,7 +5442,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>186</v>
       </c>
@@ -4767,7 +5456,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>189</v>
       </c>
@@ -4781,7 +5470,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>67</v>
       </c>
@@ -4789,7 +5478,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>226</v>
       </c>
@@ -4803,7 +5492,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>61</v>
       </c>
@@ -4817,7 +5506,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>196</v>
       </c>
@@ -4831,7 +5520,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>199</v>
       </c>
@@ -4845,7 +5534,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>202</v>
       </c>
@@ -4859,7 +5548,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>205</v>
       </c>
@@ -4873,7 +5562,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>208</v>
       </c>
@@ -4887,7 +5576,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>67</v>
       </c>
@@ -4895,7 +5584,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
         <v>227</v>
       </c>
@@ -4909,7 +5598,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>213</v>
       </c>
@@ -4923,7 +5612,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>215</v>
       </c>
@@ -4937,7 +5626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>217</v>
       </c>
@@ -4959,12 +5648,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003E7D4F9E02A40A44B19573CF3549EA08" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ace961a321deb82782cd5c0baf6e3ff0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="82b34e2e-8e49-44a7-8df8-19c48343e702" xmlns:ns3="ae66a276-7bf3-42b9-ad7d-2d219e3e493c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d6053f4621972f75917b35bd6cb2e7c" ns2:_="" ns3:_="">
     <xsd:import namespace="82b34e2e-8e49-44a7-8df8-19c48343e702"/>
@@ -5173,16 +5871,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE8075E-604D-4DFC-9C7E-787F5D4F93CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C852E5F9-ACE0-4E1C-B7EF-E70CB4A004C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -5199,7 +5896,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8463844C-F157-45FA-9070-EA9E954ADECA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5216,12 +5913,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EE8075E-604D-4DFC-9C7E-787F5D4F93CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>